<commit_message>
Subir todo el proyecto a nueva rama
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-3.125</t>
+          <t>11.125</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.388707037643208</t>
+          <t>1.33256010122311</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.88870703764321</t>
+          <t>1.16743989877689</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.842177693346846</t>
+          <t>-1.57631747829391</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.105129720534756</t>
+          <t>0.236559671274285</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.99383675817796</t>
+          <t>1.40399957005117</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.0491542264913936</t>
+          <t>-0.636414848616419</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0061442493182575</t>
+          <t>0.105985767951837</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.99998100749622</t>
+          <t>1.50998533800301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0001519385873781</t>
+          <t>-0.0671346294871952</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.89923234215073e-05</t>
+          <t>0.011293924179594</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,39 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.99999999981964</t>
+          <t>1.5212792621826</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-1.44286005352745e-09</t>
+          <t>-0.0005969755555189</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.80357506707196e-10</t>
+          <t>0.0001004368741777</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1.52137969905678</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-4.60512058374181e-08</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>7.747786634482171e-09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Subiendo cambios actuales a RamaAnderson
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>-0.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11.125</t>
+          <t>3.375</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.33256010122311</t>
+          <t>16936.2850417816</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.16743989877689</t>
+          <t>-2.95206698574524e-05</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.57631747829391</t>
+          <t>2.00008856200955</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.236559671274285</t>
+          <t>1.00004427663443</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.40399957005117</t>
+          <t>0.666732470480711</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.636414848616419</t>
+          <t>0.296186631933458</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.105985767951837</t>
+          <t>0.317399175173803</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.50998533800301</t>
+          <t>0.976753098196847</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0671346294871952</t>
+          <t>0.0016086922758489</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.011293924179594</t>
+          <t>0.0231586063769665</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.5212792621826</t>
+          <t>0.999909611297429</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-0.0005969755555189</t>
+          <t>2.45096138939971e-08</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.0001004368741777</t>
+          <t>9.19113512644414e-05</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,39 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.52137969905678</t>
+          <t>1.00000152278866</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-4.60512058374181e-08</t>
+          <t>6.95643542769631e-12</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7.747786634482171e-09</t>
+          <t>7.99779189054593e-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1.00000072300889</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.56852308919042e-12</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Grafica lineas de ecuaciones seccion 2
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,127 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11.125</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.33256010122311</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1.16743989877689</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-1.57631747829391</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.236559671274285</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1.40399957005117</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-0.636414848616419</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.105985767951837</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.50998533800301</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-0.0671346294871952</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.011293924179594</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.5212792621826</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-0.0005969755555189</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.0001004368741777</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.52137969905678</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-4.60512058374181e-08</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>7.747786634482171e-09</t>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios informe sección 1, añadir matlab informe
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-0.5</t>
+          <t>-2.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.375</t>
+          <t>-8.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16936.2850417816</t>
+          <t>2.0003606680642</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-2.95206698574524e-05</t>
+          <t>0.000360668064204</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.00008856200955</t>
+          <t>4.6916225675279003e-11</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.00004427663443</t>
+          <t>0.0003576882720103</t>
         </is>
       </c>
     </row>
@@ -507,103 +507,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.666732470480711</t>
+          <t>2.97979219374231e-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.296186631933458</t>
+          <t>2.64580561779787e-17</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t>0.317399175173803</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.976753098196847</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.0016086922758489</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.0231586063769665</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.999909611297429</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.45096138939971e-08</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>9.19113512644414e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.00000152278866</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>6.95643542769631e-12</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>7.99779189054593e-07</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1.00000072300889</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.56852308919042e-12</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
se arreglo lo de los valores en los formularios y las gráficas de los métodos, todo de la ssección 1
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-0.5</t>
+          <t>-2.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.375</t>
+          <t>-8.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16936.2850417816</t>
+          <t>2.0003606680642</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-2.95206698574524e-05</t>
+          <t>0.000360668064204</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.00008856200955</t>
+          <t>4.6916225675279003e-11</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.00004427663443</t>
+          <t>0.0003576882720103</t>
         </is>
       </c>
     </row>
@@ -507,103 +507,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.666732470480711</t>
+          <t>2.97979219374231e-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.296186631933458</t>
+          <t>2.64580561779787e-17</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t>0.317399175173803</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.976753098196847</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.0016086922758489</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.0231586063769665</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.999909611297429</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.45096138939971e-08</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>9.19113512644414e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.00000152278866</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>6.95643542769631e-12</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>7.99779189054593e-07</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1.00000072300889</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.56852308919042e-12</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>

<commit_message>
Informe 1 casi completo
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.0003606680642</t>
+          <t>1.0005</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0003576882720103</t>
+          <t>2.0003606680642</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>0.0003576882720103</t>
         </is>
       </c>
     </row>

</xml_diff>